<commit_message>
Excel sütun adı düzeltildi
</commit_message>
<xml_diff>
--- a/maillist.xlsx
+++ b/maillist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Emre Güngörmüş\weather-mail-sender\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D3C9684B-D17E-4606-9B94-8F12A72093E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E97818C-3AD2-412E-A50E-1016ABAED274}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="23520" xr2:uid="{D4A98F6C-866F-476F-BC52-E49EBDB5CAB2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{D4A98F6C-866F-476F-BC52-E49EBDB5CAB2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,12 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
-    <t>İl</t>
-  </si>
-  <si>
-    <t>Eposta</t>
-  </si>
-  <si>
     <t>Ankara</t>
   </si>
   <si>
@@ -63,6 +57,12 @@
   </si>
   <si>
     <t>uhte.erzik@gloriajeans.com.tr</t>
+  </si>
+  <si>
+    <t>sehir</t>
+  </si>
+  <si>
+    <t>email</t>
   </si>
 </sst>
 </file>
@@ -457,7 +457,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -468,42 +468,42 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>